<commit_message>
Invoke-PSImage + updating data.xlsx
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marco/Desktop/lavori/android/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marco/Desktop/Repositories/AndroidStego/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18BA6EB-87B6-4147-9E98-DE6552CF5909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1DBAAE6-98D8-9D4A-B71D-D871085BBA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="760" windowWidth="29340" windowHeight="18880" activeTab="1" xr2:uid="{9B7609F0-0CDC-D248-B70C-3CE1080E6CBB}"/>
+    <workbookView xWindow="980" yWindow="760" windowWidth="29320" windowHeight="18880" xr2:uid="{9B7609F0-0CDC-D248-B70C-3CE1080E6CBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Images" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="88">
   <si>
     <t>Type</t>
   </si>
@@ -292,6 +292,15 @@
   </si>
   <si>
     <t>png, LA</t>
+  </si>
+  <si>
+    <t>Invoke-PSImage</t>
+  </si>
+  <si>
+    <t>Tool</t>
+  </si>
+  <si>
+    <t>AudioStego</t>
   </si>
 </sst>
 </file>
@@ -327,8 +336,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -666,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC49F5D2-DCDC-0C44-A07A-D5F1EBBC2628}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -681,19 +693,20 @@
     <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D1" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -715,8 +728,11 @@
       <c r="G2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -726,14 +742,17 @@
       <c r="C3" t="s">
         <v>84</v>
       </c>
-      <c r="D3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -743,14 +762,17 @@
       <c r="C4" t="s">
         <v>84</v>
       </c>
-      <c r="D4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -760,17 +782,21 @@
       <c r="C5" t="s">
         <v>82</v>
       </c>
-      <c r="D5" t="s">
-        <v>79</v>
-      </c>
-      <c r="E5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -780,14 +806,17 @@
       <c r="C6" t="s">
         <v>84</v>
       </c>
-      <c r="D6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -797,14 +826,17 @@
       <c r="C7" t="s">
         <v>84</v>
       </c>
-      <c r="D7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -814,14 +846,19 @@
       <c r="C8" t="s">
         <v>84</v>
       </c>
-      <c r="D8" t="s">
-        <v>79</v>
-      </c>
-      <c r="E8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -831,14 +868,17 @@
       <c r="C9" t="s">
         <v>84</v>
       </c>
-      <c r="D9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D9" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -848,14 +888,19 @@
       <c r="C10" t="s">
         <v>84</v>
       </c>
-      <c r="D10" t="s">
-        <v>79</v>
-      </c>
-      <c r="E10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -865,14 +910,19 @@
       <c r="C11" t="s">
         <v>84</v>
       </c>
-      <c r="D11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -882,14 +932,17 @@
       <c r="C12" t="s">
         <v>84</v>
       </c>
-      <c r="D12" t="s">
-        <v>79</v>
-      </c>
-      <c r="E12" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -899,14 +952,17 @@
       <c r="C13" t="s">
         <v>84</v>
       </c>
-      <c r="D13" t="s">
-        <v>79</v>
-      </c>
-      <c r="E13" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D13" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -916,14 +972,17 @@
       <c r="C14" t="s">
         <v>84</v>
       </c>
-      <c r="D14" t="s">
-        <v>79</v>
-      </c>
-      <c r="E14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -933,14 +992,17 @@
       <c r="C15" t="s">
         <v>84</v>
       </c>
-      <c r="D15" t="s">
-        <v>79</v>
-      </c>
-      <c r="E15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -950,14 +1012,17 @@
       <c r="C16" t="s">
         <v>84</v>
       </c>
-      <c r="D16" t="s">
-        <v>79</v>
-      </c>
-      <c r="E16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -967,17 +1032,19 @@
       <c r="C17" t="s">
         <v>82</v>
       </c>
-      <c r="D17" t="s">
-        <v>79</v>
-      </c>
-      <c r="E17" t="s">
-        <v>79</v>
-      </c>
-      <c r="F17" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -987,14 +1054,19 @@
       <c r="C18" t="s">
         <v>83</v>
       </c>
-      <c r="D18" t="s">
-        <v>79</v>
-      </c>
-      <c r="E18" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -1004,14 +1076,19 @@
       <c r="C19" t="s">
         <v>84</v>
       </c>
-      <c r="D19" t="s">
-        <v>79</v>
-      </c>
-      <c r="E19" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -1021,14 +1098,19 @@
       <c r="C20" t="s">
         <v>84</v>
       </c>
-      <c r="D20" t="s">
-        <v>79</v>
-      </c>
-      <c r="E20" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1038,17 +1120,21 @@
       <c r="C21" t="s">
         <v>82</v>
       </c>
-      <c r="D21" t="s">
-        <v>79</v>
-      </c>
-      <c r="E21" t="s">
-        <v>79</v>
-      </c>
-      <c r="F21" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1058,14 +1144,17 @@
       <c r="C22" t="s">
         <v>84</v>
       </c>
-      <c r="D22" t="s">
-        <v>79</v>
-      </c>
-      <c r="E22" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -1075,14 +1164,17 @@
       <c r="C23" t="s">
         <v>84</v>
       </c>
-      <c r="D23" t="s">
-        <v>79</v>
-      </c>
-      <c r="E23" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D23" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -1092,14 +1184,19 @@
       <c r="C24" t="s">
         <v>84</v>
       </c>
-      <c r="D24" t="s">
-        <v>79</v>
-      </c>
-      <c r="E24" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -1109,20 +1206,23 @@
       <c r="C25" t="s">
         <v>81</v>
       </c>
-      <c r="D25" t="s">
-        <v>79</v>
-      </c>
-      <c r="E25" t="s">
-        <v>79</v>
-      </c>
-      <c r="F25" t="s">
-        <v>79</v>
-      </c>
-      <c r="G25" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D25" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1132,14 +1232,17 @@
       <c r="C26" t="s">
         <v>84</v>
       </c>
-      <c r="D26" t="s">
-        <v>79</v>
-      </c>
-      <c r="E26" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1149,14 +1252,17 @@
       <c r="C27" t="s">
         <v>84</v>
       </c>
-      <c r="D27" t="s">
-        <v>79</v>
-      </c>
-      <c r="E27" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D27" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -1166,14 +1272,19 @@
       <c r="C28" t="s">
         <v>84</v>
       </c>
-      <c r="D28" t="s">
-        <v>79</v>
-      </c>
-      <c r="E28" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -1183,17 +1294,21 @@
       <c r="C29" t="s">
         <v>82</v>
       </c>
-      <c r="D29" t="s">
-        <v>79</v>
-      </c>
-      <c r="E29" t="s">
-        <v>79</v>
-      </c>
-      <c r="F29" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D29" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -1203,20 +1318,23 @@
       <c r="C30" t="s">
         <v>81</v>
       </c>
-      <c r="D30" t="s">
-        <v>79</v>
-      </c>
-      <c r="E30" t="s">
-        <v>79</v>
-      </c>
-      <c r="F30" t="s">
-        <v>79</v>
-      </c>
-      <c r="G30" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D30" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -1226,17 +1344,21 @@
       <c r="C31" t="s">
         <v>82</v>
       </c>
-      <c r="D31" t="s">
-        <v>79</v>
-      </c>
-      <c r="E31" t="s">
-        <v>79</v>
-      </c>
-      <c r="F31" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D31" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -1246,17 +1368,21 @@
       <c r="C32" t="s">
         <v>82</v>
       </c>
-      <c r="D32" t="s">
-        <v>79</v>
-      </c>
-      <c r="E32" t="s">
-        <v>79</v>
-      </c>
-      <c r="F32" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D32" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -1266,17 +1392,21 @@
       <c r="C33" t="s">
         <v>82</v>
       </c>
-      <c r="D33" t="s">
-        <v>79</v>
-      </c>
-      <c r="E33" t="s">
-        <v>79</v>
-      </c>
-      <c r="F33" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D33" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -1286,17 +1416,21 @@
       <c r="C34" t="s">
         <v>82</v>
       </c>
-      <c r="D34" t="s">
-        <v>79</v>
-      </c>
-      <c r="E34" t="s">
-        <v>79</v>
-      </c>
-      <c r="F34" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1306,14 +1440,19 @@
       <c r="C35" t="s">
         <v>84</v>
       </c>
-      <c r="D35" t="s">
-        <v>79</v>
-      </c>
-      <c r="E35" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D35" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -1323,14 +1462,19 @@
       <c r="C36" t="s">
         <v>84</v>
       </c>
-      <c r="D36" t="s">
-        <v>79</v>
-      </c>
-      <c r="E36" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D36" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -1340,14 +1484,19 @@
       <c r="C37" t="s">
         <v>84</v>
       </c>
-      <c r="D37" t="s">
-        <v>79</v>
-      </c>
-      <c r="E37" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D37" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -1357,10 +1506,15 @@
       <c r="C38" t="s">
         <v>84</v>
       </c>
-      <c r="D38" t="s">
-        <v>79</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="D38" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1375,10 +1529,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDBB1D6C-91B2-D045-8031-B9C2E53E079D}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1386,9 +1540,10 @@
     <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1398,8 +1553,11 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1409,8 +1567,11 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1420,8 +1581,11 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1431,8 +1595,11 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1442,8 +1609,11 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1453,8 +1623,11 @@
       <c r="C6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1464,8 +1637,11 @@
       <c r="C7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1475,8 +1651,11 @@
       <c r="C8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1486,8 +1665,11 @@
       <c r="C9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -1497,8 +1679,11 @@
       <c r="C10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -1508,8 +1693,11 @@
       <c r="C11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1519,8 +1707,11 @@
       <c r="C12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1530,8 +1721,11 @@
       <c r="C13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -1541,8 +1735,11 @@
       <c r="C14" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1552,8 +1749,11 @@
       <c r="C15" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -1563,8 +1763,11 @@
       <c r="C16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -1574,8 +1777,11 @@
       <c r="C17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -1585,8 +1791,11 @@
       <c r="C18" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -1595,6 +1804,9 @@
       </c>
       <c r="C19" t="s">
         <v>20</v>
+      </c>
+      <c r="D19" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update decoding and data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marco/Desktop/Repositories/AndroidStego/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1DBAAE6-98D8-9D4A-B71D-D871085BBA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AE5540-DEBA-0444-9307-6726DE626334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="760" windowWidth="29320" windowHeight="18880" xr2:uid="{9B7609F0-0CDC-D248-B70C-3CE1080E6CBB}"/>
+    <workbookView xWindow="980" yWindow="500" windowWidth="18700" windowHeight="21100" xr2:uid="{9B7609F0-0CDC-D248-B70C-3CE1080E6CBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Images" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="88">
   <si>
     <t>Type</t>
   </si>
@@ -681,7 +681,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -785,9 +785,7 @@
       <c r="D5" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
         <v>79</v>
       </c>
@@ -1035,9 +1033,7 @@
       <c r="D17" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E17" s="1"/>
       <c r="F17" s="1" t="s">
         <v>79</v>
       </c>
@@ -1123,9 +1119,7 @@
       <c r="D21" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
         <v>79</v>
       </c>
@@ -1209,9 +1203,7 @@
       <c r="D25" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
         <v>79</v>
       </c>
@@ -1297,9 +1289,7 @@
       <c r="D29" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E29" s="1"/>
       <c r="F29" s="1" t="s">
         <v>79</v>
       </c>
@@ -1347,9 +1337,7 @@
       <c r="D31" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E31" s="1"/>
       <c r="F31" s="1" t="s">
         <v>79</v>
       </c>
@@ -1371,9 +1359,7 @@
       <c r="D32" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
         <v>79</v>
       </c>
@@ -1395,9 +1381,7 @@
       <c r="D33" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
         <v>79</v>
       </c>
@@ -1419,9 +1403,7 @@
       <c r="D34" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E34" s="1"/>
       <c r="F34" s="1" t="s">
         <v>79</v>
       </c>

</xml_diff>

<commit_message>
Final dataset + final decoding scripts
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marco/Desktop/Repositories/AndroidStego/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922B6A04-8599-254C-90DD-C737DAE32F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5652EE96-C45C-7640-AEAD-D73F0EEF588F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="500" windowWidth="18700" windowHeight="21100" xr2:uid="{9B7609F0-0CDC-D248-B70C-3CE1080E6CBB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{9B7609F0-0CDC-D248-B70C-3CE1080E6CBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Images" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="88">
   <si>
     <t>Type</t>
   </si>
@@ -681,7 +681,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:F34"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -745,9 +745,7 @@
       <c r="D3" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -765,9 +763,7 @@
       <c r="D4" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -790,9 +786,7 @@
         <v>79</v>
       </c>
       <c r="G5" s="1"/>
-      <c r="H5" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -807,9 +801,7 @@
       <c r="D6" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -827,9 +819,7 @@
       <c r="D7" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -847,14 +837,10 @@
       <c r="D8" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -869,9 +855,7 @@
       <c r="D9" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -889,14 +873,10 @@
       <c r="D10" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -911,14 +891,10 @@
       <c r="D11" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -933,9 +909,7 @@
       <c r="D12" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -953,9 +927,7 @@
       <c r="D13" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -973,9 +945,7 @@
       <c r="D14" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -993,9 +963,7 @@
       <c r="D15" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -1013,9 +981,7 @@
       <c r="D16" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -1058,9 +1024,7 @@
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -1075,14 +1039,10 @@
       <c r="D19" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
@@ -1097,14 +1057,10 @@
       <c r="D20" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -1120,13 +1076,9 @@
         <v>79</v>
       </c>
       <c r="E21" s="1"/>
-      <c r="F21" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -1141,9 +1093,7 @@
       <c r="D22" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -1161,9 +1111,7 @@
       <c r="D23" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -1181,14 +1129,10 @@
       <c r="D24" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -1212,9 +1156,7 @@
       <c r="G25" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
@@ -1229,9 +1171,7 @@
       <c r="D26" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -1249,9 +1189,7 @@
       <c r="D27" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -1269,14 +1207,10 @@
       <c r="D28" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -1296,9 +1230,7 @@
         <v>79</v>
       </c>
       <c r="G29" s="1"/>
-      <c r="H29" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
@@ -1322,9 +1254,7 @@
       <c r="G30" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -1344,9 +1274,7 @@
         <v>79</v>
       </c>
       <c r="G31" s="1"/>
-      <c r="H31" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -1366,9 +1294,7 @@
         <v>79</v>
       </c>
       <c r="G32" s="1"/>
-      <c r="H32" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
@@ -1388,9 +1314,7 @@
         <v>79</v>
       </c>
       <c r="G33" s="1"/>
-      <c r="H33" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
@@ -1410,9 +1334,7 @@
         <v>79</v>
       </c>
       <c r="G34" s="1"/>
-      <c r="H34" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
@@ -1427,14 +1349,10 @@
       <c r="D35" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-      <c r="H35" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
@@ -1449,14 +1367,10 @@
       <c r="D36" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
-      <c r="H36" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
@@ -1471,14 +1385,10 @@
       <c r="D37" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
-      <c r="H37" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
@@ -1493,14 +1403,10 @@
       <c r="D38" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
-      <c r="H38" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="H38" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>